<commit_message>
EPBDS-4379 - Update tutorials, Add examples
</commit_message>
<xml_diff>
--- a/STUDIO/trunk/org.openl.rules.demo/src/org.openl.rules.demo.tutorials/Tutorial 1 - Introduction to Decision Tables/Main.xlsx
+++ b/STUDIO/trunk/org.openl.rules.demo/src/org.openl.rules.demo.tutorials/Tutorial 1 - Introduction to Decision Tables/Main.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_st33">Step3!$C$63</definedName>
     <definedName name="_st34">Step3!$C$105</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525" calcMode="manual" iterate="1" iterateCount="1000"/>
 </workbook>
 </file>
 
@@ -216,7 +216,8 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>This rule is interpreted as if the hour from 12am till 5pm then greeting is "Good Afternoon, World!"</t>
+          <t>This rule is interpreted as if the hour from 12 till 17
+ o'clock then greeting is "Good Afternoon, World!"</t>
         </r>
       </text>
     </comment>
@@ -491,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="118">
   <si>
     <t>Rule</t>
   </si>
@@ -554,9 +555,6 @@
     <t>driverAge</t>
   </si>
   <si>
-    <t>driverMS</t>
-  </si>
-  <si>
     <t>Driver Age</t>
   </si>
   <si>
@@ -819,9 +817,6 @@
     <t>HC1</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>String</t>
   </si>
   <si>
@@ -844,92 +839,6 @@
   </si>
   <si>
     <t>Step2. Lookup Table and its structure</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">            A </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Lookup table</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> is a Decision table which contains both vertical and horizontal conditions and returns value on crossroads of matching condition values.
-            Lookup table must have:
-• at least one </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>vertical condition (C)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">;
-• at least one </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>horizontal condition (HC)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">. Please, note that HC columns do not have Titles section (display names);
-• exactly </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>one return column (RET)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>.
-            Let's present rules table DriverPremiumInc in Lookup table format which is the most compact for such kind of rules:</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1046,9 +955,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">           P.S. All tables DriverPremiumInc_%, presented in different table formats, produce the same result.</t>
-  </si>
-  <si>
     <t>Step2-2. Lookup Table with several horizontal conditions</t>
   </si>
   <si>
@@ -1234,90 +1140,6 @@
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">            A </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>decision table</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> is a set of rules describing decision situations where the state of a number of conditions determines the execution of a set of actions. It is the basic table type used in OpenL Tablets decision making. 
-            </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Rules inside decision tables are processed one by one in the order they are placed in the table</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">.
-           </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>A rule is executed only when all its conditions are true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>. Absence of a parameter in a condition cell is interpreted as a true value. Blank action/return value cells are ignored. Decision table</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> returns the first not blank value </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>of the rule row rules whose conditions are true. 
-The following is an example of Decision table determining  appropriate Greeting according to current hours:</t>
     </r>
   </si>
   <si>
@@ -1411,7 +1233,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Rules DoubleValue </t>
+      <t xml:space="preserve">Rules String </t>
     </r>
     <r>
       <rPr>
@@ -1421,7 +1243,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium1</t>
+      <t>Greeting1</t>
     </r>
     <r>
       <rPr>
@@ -1431,12 +1253,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverMS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules DoubleValue </t>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules String </t>
     </r>
     <r>
       <rPr>
@@ -1446,7 +1268,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium2</t>
+      <t>Greeting2</t>
     </r>
     <r>
       <rPr>
@@ -1456,12 +1278,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverMS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules DoubleValue </t>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules String </t>
     </r>
     <r>
       <rPr>
@@ -1471,7 +1293,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium3</t>
+      <t>Greeting3</t>
     </r>
     <r>
       <rPr>
@@ -1481,12 +1303,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverMS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules DoubleValue </t>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules String </t>
     </r>
     <r>
       <rPr>
@@ -1496,7 +1318,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium4</t>
+      <t>Greeting4</t>
     </r>
     <r>
       <rPr>
@@ -1506,12 +1328,18 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverMS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleLookup DoubleValue </t>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">            P.S.You may notice that sets of tables Greeting[N] or DriverPremium[N] produce the same result, the logic part of rules stays the same. </t>
+  </si>
+  <si>
+    <t>driverMaritalStatus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules DoubleValue </t>
     </r>
     <r>
       <rPr>
@@ -1521,7 +1349,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium5</t>
+      <t>DriverPremium1</t>
     </r>
     <r>
       <rPr>
@@ -1531,12 +1359,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (String driverAge, String driverMS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules String </t>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules DoubleValue </t>
     </r>
     <r>
       <rPr>
@@ -1546,7 +1374,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>Greeting1</t>
+      <t>DriverPremium2</t>
     </r>
     <r>
       <rPr>
@@ -1556,12 +1384,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules String </t>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleLookup DoubleValue </t>
     </r>
     <r>
       <rPr>
@@ -1571,7 +1399,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>Greeting2</t>
+      <t>DriverPremium5</t>
     </r>
     <r>
       <rPr>
@@ -1581,12 +1409,101 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules String </t>
+      <t xml:space="preserve"> (String driverAge, String driverdriverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Lookup table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> is a Decision table which contains both vertical and horizontal conditions and returns value on crossroads of matching condition values.
+            Lookup table must have:
+• at least one </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>vertical condition (C)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">;
+• at least one </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>horizontal condition (HC)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">. Please, note that HC columns do not have Titles section (display names);
+• exactly </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>one return column (RET)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>.
+            Let's present rules table DriverPremium in Lookup table format which is the most compact for such kind of rules:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">           P.S. All tables DriverPremium, presented in different table formats, produce the same result.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules void </t>
     </r>
     <r>
       <rPr>
@@ -1596,7 +1513,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>Greeting3</t>
+      <t>Greeting5</t>
     </r>
     <r>
       <rPr>
@@ -1611,7 +1528,91 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">SimpleRules String </t>
+      <t xml:space="preserve">            A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>decision table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> is a set of rules describing decision situations where the state of a number of conditions determines the execution of a set of actions. It is the basic table type used in OpenL Tablets decision making. 
+            </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Rules inside decision tables are processed from top to bottom one by one </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+           </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>A rule is executed only when all its conditions are true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>. Absence of a parameter in a condition cell is interpreted as a true value. Blank action/return value cells are ignored. Decision table</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> returns the first not blank value </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>of the rule row rules whose conditions are true. 
+The following is an example of Decision table determining  appropriate Greeting according to current hours:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules DoubleValue </t>
     </r>
     <r>
       <rPr>
@@ -1621,7 +1622,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>Greeting4</t>
+      <t>DriverPremium3</t>
     </r>
     <r>
       <rPr>
@@ -1631,12 +1632,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules void </t>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules DoubleValue </t>
     </r>
     <r>
       <rPr>
@@ -1646,7 +1647,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>Greeting6</t>
+      <t>DriverPremium4</t>
     </r>
     <r>
       <rPr>
@@ -1656,11 +1657,11 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">            P.S.You may notice that sets of tables Greeting[N] or DriverPremium[N] produce the same result, the logic part of rules stays the same. </t>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -1672,7 +1673,7 @@
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
     <numFmt numFmtId="165" formatCode="\ &quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2221,7 +2222,7 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2376,9 +2377,6 @@
     <xf numFmtId="165" fontId="4" fillId="5" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2398,9 +2396,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2410,6 +2405,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2482,6 +2481,9 @@
     <xf numFmtId="165" fontId="4" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2496,18 +2498,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 5" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC91D"/>
       <color rgb="FFFEFCCE"/>
       <color rgb="FFFDFAB9"/>
       <color rgb="FFF0DB5E"/>
-      <color rgb="FFFFC91D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2998,18 +3000,18 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="9" width="9.140625" style="3" collapsed="1"/>
     <col min="10" max="10" width="19.140625" style="3" customWidth="1" collapsed="1"/>
     <col min="11" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="21" thickBot="1">
       <c r="B3" s="70" t="s">
         <v>17</v>
       </c>
@@ -3021,14 +3023,14 @@
       <c r="H3" s="70"/>
       <c r="I3" s="70"/>
     </row>
-    <row r="4" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="13.5" thickTop="1">
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="43"/>
       <c r="G4" s="43"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3040,7 +3042,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="13.5" thickBot="1">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -3052,7 +3054,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="12.75" customHeight="1">
       <c r="B8" s="4"/>
       <c r="C8" s="73" t="s">
         <v>18</v>
@@ -3066,7 +3068,7 @@
       <c r="J8" s="74"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="12.75" customHeight="1">
       <c r="B9" s="4"/>
       <c r="C9" s="75"/>
       <c r="D9" s="75"/>
@@ -3078,7 +3080,7 @@
       <c r="J9" s="75"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="13.5" customHeight="1">
       <c r="B10" s="4"/>
       <c r="C10" s="75"/>
       <c r="D10" s="75"/>
@@ -3090,7 +3092,7 @@
       <c r="J10" s="75"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="12.75" customHeight="1">
       <c r="B11" s="4"/>
       <c r="C11" s="75"/>
       <c r="D11" s="75"/>
@@ -3102,7 +3104,7 @@
       <c r="J11" s="75"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="12.75" customHeight="1">
       <c r="B12" s="4"/>
       <c r="C12" s="75"/>
       <c r="D12" s="75"/>
@@ -3114,7 +3116,7 @@
       <c r="J12" s="75"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="12.75" customHeight="1">
       <c r="B13" s="4"/>
       <c r="C13" s="75"/>
       <c r="D13" s="75"/>
@@ -3126,7 +3128,7 @@
       <c r="J13" s="75"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="12.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="75"/>
       <c r="D14" s="75"/>
@@ -3138,7 +3140,7 @@
       <c r="J14" s="75"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="12.75" customHeight="1">
       <c r="B15" s="4"/>
       <c r="C15" s="75"/>
       <c r="D15" s="75"/>
@@ -3150,7 +3152,7 @@
       <c r="J15" s="75"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="12.75" customHeight="1">
       <c r="B16" s="4"/>
       <c r="C16" s="75"/>
       <c r="D16" s="75"/>
@@ -3162,7 +3164,7 @@
       <c r="J16" s="75"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="12.75" customHeight="1">
       <c r="B17" s="4"/>
       <c r="C17" s="75"/>
       <c r="D17" s="75"/>
@@ -3174,7 +3176,7 @@
       <c r="J17" s="75"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" s="11" customFormat="1" ht="12.75" customHeight="1">
       <c r="B18" s="12"/>
       <c r="C18" s="75"/>
       <c r="D18" s="75"/>
@@ -3186,7 +3188,7 @@
       <c r="J18" s="75"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="12.75" customHeight="1">
       <c r="B19" s="4"/>
       <c r="C19" s="75"/>
       <c r="D19" s="75"/>
@@ -3198,7 +3200,7 @@
       <c r="J19" s="75"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="12.75" customHeight="1">
       <c r="B20" s="4"/>
       <c r="C20" s="75"/>
       <c r="D20" s="75"/>
@@ -3210,7 +3212,7 @@
       <c r="J20" s="75"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="12.75" customHeight="1">
       <c r="B21" s="4"/>
       <c r="C21" s="75"/>
       <c r="D21" s="75"/>
@@ -3222,7 +3224,7 @@
       <c r="J21" s="75"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="12.75" customHeight="1" thickBot="1">
       <c r="B22" s="4"/>
       <c r="C22" s="76"/>
       <c r="D22" s="76"/>
@@ -3234,7 +3236,7 @@
       <c r="J22" s="76"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="12.75" customHeight="1">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3246,7 +3248,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="13.5" customHeight="1">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3258,7 +3260,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="13.5" customHeight="1">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3270,7 +3272,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="13.5" customHeight="1">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -3282,7 +3284,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="13.5" customHeight="1">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -3294,10 +3296,10 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="17.25" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="77" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="77"/>
       <c r="E28" s="77"/>
@@ -3308,10 +3310,10 @@
       <c r="J28" s="77"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1">
       <c r="B29" s="12"/>
       <c r="C29" s="71" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D29" s="71"/>
       <c r="E29" s="71"/>
@@ -3322,10 +3324,10 @@
       <c r="J29" s="71"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="17.25" customHeight="1">
       <c r="B30" s="4"/>
       <c r="C30" s="71" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D30" s="71"/>
       <c r="E30" s="71"/>
@@ -3336,10 +3338,10 @@
       <c r="J30" s="71"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="17.25" customHeight="1">
       <c r="B31" s="4"/>
       <c r="C31" s="71" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D31" s="71"/>
       <c r="E31" s="71"/>
@@ -3350,10 +3352,10 @@
       <c r="J31" s="71"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="17.25" customHeight="1">
       <c r="B32" s="4"/>
       <c r="C32" s="71" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
@@ -3364,10 +3366,10 @@
       <c r="J32" s="71"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1">
       <c r="B33" s="12"/>
       <c r="C33" s="71" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D33" s="71"/>
       <c r="E33" s="71"/>
@@ -3378,10 +3380,10 @@
       <c r="J33" s="71"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1">
       <c r="B34" s="12"/>
       <c r="C34" s="71" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D34" s="71"/>
       <c r="E34" s="71"/>
@@ -3392,10 +3394,10 @@
       <c r="J34" s="71"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" s="11" customFormat="1" ht="17.25" customHeight="1">
       <c r="B35" s="12"/>
       <c r="C35" s="71" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
@@ -3406,10 +3408,10 @@
       <c r="J35" s="71"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" s="4"/>
       <c r="C36" s="71" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D36" s="71"/>
       <c r="E36" s="71"/>
@@ -3420,10 +3422,10 @@
       <c r="J36" s="71"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" s="4"/>
       <c r="C37" s="72" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D37" s="72"/>
       <c r="E37" s="72"/>
@@ -3434,7 +3436,7 @@
       <c r="J37" s="72"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" s="11" customFormat="1">
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -3446,7 +3448,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" s="11" customFormat="1">
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -3458,7 +3460,7 @@
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="2:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" s="11" customFormat="1">
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -3509,41 +3511,41 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105:F105"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="8.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.140625" style="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="39.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:7" s="3" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" s="3" customFormat="1"/>
+    <row r="2" spans="2:7" s="3" customFormat="1"/>
+    <row r="3" spans="2:7" s="3" customFormat="1" ht="18.75" thickBot="1">
       <c r="B3" s="78" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
       <c r="E3" s="78"/>
       <c r="F3" s="78"/>
     </row>
-    <row r="4" spans="2:7" s="3" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" s="3" customFormat="1" ht="13.5" thickTop="1">
       <c r="B4" s="6"/>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" s="3" customFormat="1"/>
+    <row r="6" spans="2:7" s="3" customFormat="1">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -3551,7 +3553,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="2:7" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -3559,17 +3561,17 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" s="3" customFormat="1">
       <c r="B8" s="7"/>
       <c r="C8" s="80" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="80"/>
       <c r="E8" s="80"/>
       <c r="F8" s="80"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="2:7" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="B9" s="7"/>
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
@@ -3577,15 +3579,15 @@
       <c r="F9" s="81"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" s="3" customFormat="1">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="68"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" s="3" customFormat="1">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -3593,17 +3595,17 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" s="3" customFormat="1">
       <c r="B12" s="7"/>
       <c r="C12" s="84" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
       <c r="F12" s="84"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" s="3" customFormat="1">
       <c r="B13" s="7"/>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
@@ -3611,7 +3613,7 @@
       <c r="F13" s="85"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" s="3" customFormat="1">
       <c r="B14" s="7"/>
       <c r="C14" s="85"/>
       <c r="D14" s="85"/>
@@ -3619,7 +3621,7 @@
       <c r="F14" s="85"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" s="11" customFormat="1">
       <c r="B15" s="9"/>
       <c r="C15" s="85"/>
       <c r="D15" s="85"/>
@@ -3627,7 +3629,7 @@
       <c r="F15" s="85"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" s="11" customFormat="1">
       <c r="B16" s="9"/>
       <c r="C16" s="85"/>
       <c r="D16" s="85"/>
@@ -3635,7 +3637,7 @@
       <c r="F16" s="85"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" s="11" customFormat="1">
       <c r="B17" s="9"/>
       <c r="C17" s="85"/>
       <c r="D17" s="85"/>
@@ -3643,7 +3645,7 @@
       <c r="F17" s="85"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" s="11" customFormat="1">
       <c r="B18" s="12"/>
       <c r="C18" s="85"/>
       <c r="D18" s="85"/>
@@ -3651,7 +3653,7 @@
       <c r="F18" s="85"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" s="11" customFormat="1">
       <c r="B19" s="12"/>
       <c r="C19" s="85"/>
       <c r="D19" s="85"/>
@@ -3659,7 +3661,7 @@
       <c r="F19" s="85"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" s="11" customFormat="1">
       <c r="B20" s="12"/>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
@@ -3667,7 +3669,7 @@
       <c r="F20" s="85"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" s="11" customFormat="1">
       <c r="B21" s="9"/>
       <c r="C21" s="85"/>
       <c r="D21" s="85"/>
@@ -3675,7 +3677,7 @@
       <c r="F21" s="85"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" s="3" customFormat="1" ht="98.25" customHeight="1">
       <c r="B22" s="7"/>
       <c r="C22" s="86"/>
       <c r="D22" s="86"/>
@@ -3683,7 +3685,7 @@
       <c r="F22" s="86"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="2:7" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" s="3" customFormat="1">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -3691,7 +3693,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" s="8" customFormat="1">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -3699,31 +3701,31 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="2:7" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" s="8" customFormat="1" ht="15.75">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="79" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E25" s="79"/>
       <c r="F25" s="79"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="2:7" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" s="8" customFormat="1" ht="25.5">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>40</v>
-      </c>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" s="8" customFormat="1">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13" t="s">
@@ -3737,7 +3739,7 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" s="8" customFormat="1">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="13" t="s">
@@ -3751,21 +3753,21 @@
       </c>
       <c r="G28" s="12"/>
     </row>
-    <row r="29" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" s="8" customFormat="1">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="2:7" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="15" t="s">
@@ -3779,7 +3781,7 @@
       </c>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="2:7" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="16">
@@ -3793,7 +3795,7 @@
       </c>
       <c r="G31" s="12"/>
     </row>
-    <row r="32" spans="2:7" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" s="8" customFormat="1">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="17">
@@ -3807,7 +3809,7 @@
       </c>
       <c r="G32" s="12"/>
     </row>
-    <row r="33" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" s="8" customFormat="1">
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="17">
@@ -3821,7 +3823,7 @@
       </c>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="2:14" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="19">
@@ -3835,7 +3837,7 @@
       </c>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="2:14" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -3843,7 +3845,7 @@
       <c r="F35" s="47"/>
       <c r="G35" s="12"/>
     </row>
-    <row r="36" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" s="3" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -3851,17 +3853,17 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" s="3" customFormat="1">
       <c r="B37" s="7"/>
       <c r="C37" s="84" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="84"/>
       <c r="E37" s="84"/>
       <c r="F37" s="84"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" s="11" customFormat="1">
       <c r="B38" s="9"/>
       <c r="C38" s="85"/>
       <c r="D38" s="85"/>
@@ -3869,7 +3871,7 @@
       <c r="F38" s="85"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" s="11" customFormat="1">
       <c r="B39" s="9"/>
       <c r="C39" s="85"/>
       <c r="D39" s="85"/>
@@ -3877,7 +3879,7 @@
       <c r="F39" s="85"/>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" s="11" customFormat="1">
       <c r="B40" s="9"/>
       <c r="C40" s="85"/>
       <c r="D40" s="85"/>
@@ -3885,7 +3887,7 @@
       <c r="F40" s="85"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" s="11" customFormat="1">
       <c r="B41" s="9"/>
       <c r="C41" s="85"/>
       <c r="D41" s="85"/>
@@ -3893,7 +3895,7 @@
       <c r="F41" s="85"/>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" s="11" customFormat="1">
       <c r="B42" s="9"/>
       <c r="C42" s="85"/>
       <c r="D42" s="85"/>
@@ -3901,7 +3903,7 @@
       <c r="F42" s="85"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" s="11" customFormat="1">
       <c r="B43" s="9"/>
       <c r="C43" s="85"/>
       <c r="D43" s="85"/>
@@ -3909,7 +3911,7 @@
       <c r="F43" s="85"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" s="11" customFormat="1">
       <c r="B44" s="9"/>
       <c r="C44" s="85"/>
       <c r="D44" s="85"/>
@@ -3917,7 +3919,7 @@
       <c r="F44" s="85"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="2:14" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" s="11" customFormat="1">
       <c r="B45" s="9"/>
       <c r="C45" s="85"/>
       <c r="D45" s="85"/>
@@ -3925,7 +3927,7 @@
       <c r="F45" s="85"/>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" s="3" customFormat="1">
       <c r="B46" s="7"/>
       <c r="C46" s="85"/>
       <c r="D46" s="85"/>
@@ -3933,7 +3935,7 @@
       <c r="F46" s="85"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" s="3" customFormat="1">
       <c r="B47" s="7"/>
       <c r="C47" s="86"/>
       <c r="D47" s="86"/>
@@ -3944,7 +3946,7 @@
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
     </row>
-    <row r="48" spans="2:14" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" s="3" customFormat="1">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -3955,7 +3957,7 @@
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
     </row>
-    <row r="49" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" s="11" customFormat="1">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -3963,17 +3965,17 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" s="11" customFormat="1">
       <c r="B50" s="9"/>
       <c r="C50" s="84" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D50" s="84"/>
       <c r="E50" s="84"/>
       <c r="F50" s="84"/>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" s="11" customFormat="1">
       <c r="B51" s="9"/>
       <c r="C51" s="85"/>
       <c r="D51" s="85"/>
@@ -3981,7 +3983,7 @@
       <c r="F51" s="85"/>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" s="11" customFormat="1">
       <c r="B52" s="9"/>
       <c r="C52" s="85"/>
       <c r="D52" s="85"/>
@@ -3989,7 +3991,7 @@
       <c r="F52" s="85"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" s="11" customFormat="1">
       <c r="B53" s="9"/>
       <c r="C53" s="85"/>
       <c r="D53" s="85"/>
@@ -3997,7 +3999,7 @@
       <c r="F53" s="85"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" s="11" customFormat="1">
       <c r="B54" s="9"/>
       <c r="C54" s="86"/>
       <c r="D54" s="86"/>
@@ -4005,7 +4007,7 @@
       <c r="F54" s="86"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" s="11" customFormat="1">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -4013,7 +4015,7 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" s="11" customFormat="1">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -4021,17 +4023,17 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="2:13" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:13" ht="15.75">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="79" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E57" s="79"/>
       <c r="F57" s="79"/>
       <c r="G57" s="12"/>
     </row>
-    <row r="58" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:13">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="13" t="s">
@@ -4045,80 +4047,80 @@
       </c>
       <c r="G58" s="12"/>
     </row>
-    <row r="59" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:13">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="39" t="s">
         <v>19</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F59" s="13"/>
       <c r="G59" s="12"/>
     </row>
-    <row r="60" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:13">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F60" s="13"/>
       <c r="G60" s="12"/>
     </row>
-    <row r="61" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" ht="13.5" thickBot="1">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E61" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="F61" s="45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="2:13" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:13" ht="13.5" thickTop="1">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="F62" s="48">
         <v>700</v>
       </c>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:13">
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F63" s="20">
         <v>720</v>
       </c>
       <c r="G63" s="12"/>
     </row>
-    <row r="64" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:13">
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
       <c r="D64" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F64" s="20">
         <v>300</v>
@@ -4126,14 +4128,14 @@
       <c r="G64" s="12"/>
       <c r="M64" s="10"/>
     </row>
-    <row r="65" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:13">
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F65" s="20">
         <v>350</v>
@@ -4141,11 +4143,11 @@
       <c r="G65" s="12"/>
       <c r="M65" s="10"/>
     </row>
-    <row r="66" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" ht="13.5" thickBot="1">
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E66" s="21"/>
       <c r="F66" s="49">
@@ -4154,7 +4156,7 @@
       <c r="G66" s="12"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="67" spans="2:13" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:13" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -4162,7 +4164,7 @@
       <c r="F67" s="47"/>
       <c r="G67" s="12"/>
     </row>
-    <row r="68" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" s="11" customFormat="1">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
@@ -4170,7 +4172,7 @@
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
     </row>
-    <row r="69" spans="2:13" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" s="11" customFormat="1">
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
@@ -4178,17 +4180,17 @@
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
     </row>
-    <row r="70" spans="2:13" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" ht="15.75">
       <c r="B70" s="12"/>
       <c r="C70" s="79" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D70" s="79"/>
       <c r="E70" s="79"/>
       <c r="F70" s="79"/>
       <c r="G70" s="12"/>
     </row>
-    <row r="71" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13">
       <c r="B71" s="12"/>
       <c r="C71" s="13" t="s">
         <v>0</v>
@@ -4204,58 +4206,58 @@
       </c>
       <c r="G71" s="12"/>
     </row>
-    <row r="72" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13">
       <c r="B72" s="12"/>
       <c r="C72" s="13"/>
       <c r="D72" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F72" s="13"/>
       <c r="G72" s="12"/>
     </row>
-    <row r="73" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13">
       <c r="B73" s="12"/>
       <c r="C73" s="13"/>
       <c r="D73" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F73" s="13"/>
       <c r="G73" s="12"/>
       <c r="L73" s="10"/>
     </row>
-    <row r="74" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:13" ht="13.5" thickBot="1">
       <c r="B74" s="12"/>
       <c r="C74" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D74" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E74" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="F74" s="45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G74" s="12"/>
       <c r="L74" s="8"/>
     </row>
-    <row r="75" spans="2:13" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:13" ht="13.5" thickTop="1">
       <c r="B75" s="12"/>
       <c r="C75" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D75" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="23" t="s">
         <v>23</v>
-      </c>
-      <c r="E75" s="23" t="s">
-        <v>24</v>
       </c>
       <c r="F75" s="50">
         <v>700</v>
@@ -4263,14 +4265,14 @@
       <c r="G75" s="12"/>
       <c r="L75" s="8"/>
     </row>
-    <row r="76" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:13">
       <c r="B76" s="12"/>
       <c r="C76" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D76" s="82"/>
       <c r="E76" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F76" s="26">
         <v>720</v>
@@ -4278,16 +4280,16 @@
       <c r="G76" s="12"/>
       <c r="L76" s="8"/>
     </row>
-    <row r="77" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:13">
       <c r="B77" s="12"/>
       <c r="C77" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D77" s="82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E77" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F77" s="26">
         <v>300</v>
@@ -4295,14 +4297,14 @@
       <c r="G77" s="12"/>
       <c r="L77" s="8"/>
     </row>
-    <row r="78" spans="2:13" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13">
       <c r="B78" s="12"/>
       <c r="C78" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D78" s="82"/>
       <c r="E78" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F78" s="26">
         <v>350</v>
@@ -4310,13 +4312,13 @@
       <c r="G78" s="12"/>
       <c r="L78" s="8"/>
     </row>
-    <row r="79" spans="2:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:13" ht="13.5" thickBot="1">
       <c r="B79" s="12"/>
       <c r="C79" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E79" s="28"/>
       <c r="F79" s="51">
@@ -4324,7 +4326,7 @@
       </c>
       <c r="G79" s="12"/>
     </row>
-    <row r="80" spans="2:13" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:13" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -4332,7 +4334,7 @@
       <c r="F80" s="47"/>
       <c r="G80" s="12"/>
     </row>
-    <row r="81" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="11" customFormat="1">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -4340,7 +4342,7 @@
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
     </row>
-    <row r="82" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" s="11" customFormat="1">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
@@ -4348,17 +4350,17 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="11" customFormat="1">
       <c r="B83" s="9"/>
       <c r="C83" s="84" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D83" s="84"/>
       <c r="E83" s="84"/>
       <c r="F83" s="84"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" s="11" customFormat="1">
       <c r="B84" s="9"/>
       <c r="C84" s="86"/>
       <c r="D84" s="86"/>
@@ -4366,7 +4368,7 @@
       <c r="F84" s="86"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" s="11" customFormat="1">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
@@ -4374,7 +4376,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" s="11" customFormat="1">
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -4382,7 +4384,7 @@
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
     </row>
-    <row r="87" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" s="11" customFormat="1">
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -4390,7 +4392,7 @@
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
     </row>
-    <row r="88" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" s="11" customFormat="1">
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -4398,7 +4400,7 @@
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
     </row>
-    <row r="89" spans="1:7" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
@@ -4406,26 +4408,26 @@
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
     </row>
-    <row r="90" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15" thickBot="1">
       <c r="A90" s="8"/>
       <c r="B90" s="12"/>
       <c r="C90" s="87" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D90" s="87"/>
       <c r="E90" s="87"/>
       <c r="F90" s="87"/>
       <c r="G90" s="12"/>
     </row>
-    <row r="91" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" s="11" customFormat="1">
       <c r="B91" s="12"/>
-      <c r="C91" s="69"/>
-      <c r="D91" s="69"/>
-      <c r="E91" s="69"/>
-      <c r="F91" s="69"/>
+      <c r="C91" s="67"/>
+      <c r="D91" s="67"/>
+      <c r="E91" s="67"/>
+      <c r="F91" s="67"/>
       <c r="G91" s="12"/>
     </row>
-    <row r="92" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" s="11" customFormat="1">
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -4433,17 +4435,17 @@
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
     </row>
-    <row r="93" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" s="11" customFormat="1">
       <c r="B93" s="12"/>
       <c r="C93" s="84" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D93" s="84"/>
       <c r="E93" s="84"/>
       <c r="F93" s="84"/>
       <c r="G93" s="12"/>
     </row>
-    <row r="94" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" s="11" customFormat="1">
       <c r="B94" s="12"/>
       <c r="C94" s="85"/>
       <c r="D94" s="85"/>
@@ -4451,7 +4453,7 @@
       <c r="F94" s="85"/>
       <c r="G94" s="12"/>
     </row>
-    <row r="95" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="11" customFormat="1">
       <c r="B95" s="12"/>
       <c r="C95" s="85"/>
       <c r="D95" s="85"/>
@@ -4459,7 +4461,7 @@
       <c r="F95" s="85"/>
       <c r="G95" s="12"/>
     </row>
-    <row r="96" spans="1:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="11" customFormat="1">
       <c r="B96" s="12"/>
       <c r="C96" s="85"/>
       <c r="D96" s="85"/>
@@ -4467,7 +4469,7 @@
       <c r="F96" s="85"/>
       <c r="G96" s="12"/>
     </row>
-    <row r="97" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" s="11" customFormat="1">
       <c r="B97" s="12"/>
       <c r="C97" s="85"/>
       <c r="D97" s="85"/>
@@ -4475,7 +4477,7 @@
       <c r="F97" s="85"/>
       <c r="G97" s="12"/>
     </row>
-    <row r="98" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" s="11" customFormat="1">
       <c r="B98" s="12"/>
       <c r="C98" s="85"/>
       <c r="D98" s="85"/>
@@ -4483,7 +4485,7 @@
       <c r="F98" s="85"/>
       <c r="G98" s="12"/>
     </row>
-    <row r="99" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" s="11" customFormat="1">
       <c r="B99" s="12"/>
       <c r="C99" s="85"/>
       <c r="D99" s="85"/>
@@ -4491,7 +4493,7 @@
       <c r="F99" s="85"/>
       <c r="G99" s="12"/>
     </row>
-    <row r="100" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" s="11" customFormat="1">
       <c r="B100" s="12"/>
       <c r="C100" s="85"/>
       <c r="D100" s="85"/>
@@ -4499,7 +4501,7 @@
       <c r="F100" s="85"/>
       <c r="G100" s="12"/>
     </row>
-    <row r="101" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" s="11" customFormat="1">
       <c r="B101" s="12"/>
       <c r="C101" s="85"/>
       <c r="D101" s="85"/>
@@ -4507,7 +4509,7 @@
       <c r="F101" s="85"/>
       <c r="G101" s="12"/>
     </row>
-    <row r="102" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" s="11" customFormat="1">
       <c r="B102" s="12"/>
       <c r="C102" s="86"/>
       <c r="D102" s="86"/>
@@ -4515,7 +4517,7 @@
       <c r="F102" s="86"/>
       <c r="G102" s="12"/>
     </row>
-    <row r="103" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" s="11" customFormat="1">
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
@@ -4523,7 +4525,7 @@
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
     </row>
-    <row r="104" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" s="11" customFormat="1">
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
@@ -4531,91 +4533,91 @@
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
     </row>
-    <row r="105" spans="2:7" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" s="11" customFormat="1" ht="15.75">
       <c r="B105" s="12"/>
       <c r="C105" s="12"/>
       <c r="D105" s="79" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E105" s="79"/>
       <c r="F105" s="79"/>
       <c r="G105" s="12"/>
     </row>
-    <row r="106" spans="2:7" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:7" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
       <c r="D106" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E106" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E106" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="F106" s="45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G106" s="12"/>
     </row>
-    <row r="107" spans="2:7" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
       <c r="D107" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E107" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="E107" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="F107" s="48">
         <v>700</v>
       </c>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" s="11" customFormat="1">
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
       <c r="D108" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F108" s="20">
         <v>720</v>
       </c>
       <c r="G108" s="12"/>
     </row>
-    <row r="109" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" s="11" customFormat="1">
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
       <c r="D109" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F109" s="20">
         <v>300</v>
       </c>
       <c r="G109" s="12"/>
     </row>
-    <row r="110" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" s="11" customFormat="1">
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
       <c r="D110" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E110" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F110" s="20">
         <v>350</v>
       </c>
       <c r="G110" s="12"/>
     </row>
-    <row r="111" spans="2:7" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:7" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
       <c r="D111" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E111" s="21"/>
       <c r="F111" s="49">
@@ -4623,7 +4625,7 @@
       </c>
       <c r="G111" s="12"/>
     </row>
-    <row r="112" spans="2:7" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
@@ -4631,7 +4633,7 @@
       <c r="F112" s="47"/>
       <c r="G112" s="12"/>
     </row>
-    <row r="113" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" s="11" customFormat="1">
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
@@ -4639,7 +4641,7 @@
       <c r="F113" s="12"/>
       <c r="G113" s="12"/>
     </row>
-    <row r="114" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" s="11" customFormat="1">
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
       <c r="D114" s="12"/>
@@ -4647,7 +4649,7 @@
       <c r="F114" s="12"/>
       <c r="G114" s="12"/>
     </row>
-    <row r="115" spans="2:7" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" s="11" customFormat="1" ht="15">
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
       <c r="D115" s="34" t="s">
@@ -4657,7 +4659,7 @@
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
     </row>
-    <row r="116" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" s="11" customFormat="1">
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
       <c r="D116" s="12"/>
@@ -4665,7 +4667,7 @@
       <c r="F116" s="12"/>
       <c r="G116" s="12"/>
     </row>
-    <row r="117" spans="2:7" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" s="11" customFormat="1">
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
       <c r="D117" s="12"/>
@@ -4706,41 +4708,42 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="8" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" style="8" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="9.140625" style="8" collapsed="1"/>
+    <col min="3" max="3" width="7.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="55.42578125" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="14.28515625" style="8" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16.140625" style="8" customWidth="1" collapsed="1"/>
     <col min="9" max="16384" width="9.140625" style="8" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:9" s="11" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" s="11" customFormat="1"/>
+    <row r="2" spans="2:9" s="11" customFormat="1"/>
+    <row r="3" spans="2:9" s="11" customFormat="1" ht="18.75" thickBot="1">
       <c r="B3" s="78" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
       <c r="E3" s="78"/>
       <c r="F3" s="88"/>
     </row>
-    <row r="4" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-    </row>
-    <row r="5" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" s="11" customFormat="1" ht="13.5" thickTop="1">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+    </row>
+    <row r="5" spans="2:9" s="11" customFormat="1"/>
+    <row r="6" spans="2:9" s="11" customFormat="1">
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -4750,7 +4753,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -4760,10 +4763,10 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" s="11" customFormat="1">
       <c r="B8" s="12"/>
       <c r="C8" s="80" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="80"/>
       <c r="E8" s="80"/>
@@ -4772,7 +4775,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B9" s="12"/>
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
@@ -4782,7 +4785,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" s="11" customFormat="1">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -4792,7 +4795,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" s="11" customFormat="1">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -4802,10 +4805,10 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" s="11" customFormat="1">
       <c r="B12" s="12"/>
       <c r="C12" s="84" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
@@ -4814,7 +4817,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" s="11" customFormat="1">
       <c r="B13" s="12"/>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
@@ -4824,7 +4827,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" s="11" customFormat="1">
       <c r="B14" s="12"/>
       <c r="C14" s="85"/>
       <c r="D14" s="85"/>
@@ -4834,7 +4837,7 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" s="11" customFormat="1">
       <c r="B15" s="12"/>
       <c r="C15" s="85"/>
       <c r="D15" s="85"/>
@@ -4844,7 +4847,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" s="11" customFormat="1">
       <c r="B16" s="12"/>
       <c r="C16" s="85"/>
       <c r="D16" s="85"/>
@@ -4854,7 +4857,7 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" s="11" customFormat="1">
       <c r="B17" s="12"/>
       <c r="C17" s="85"/>
       <c r="D17" s="85"/>
@@ -4864,7 +4867,7 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" s="11" customFormat="1">
       <c r="B18" s="12"/>
       <c r="C18" s="85"/>
       <c r="D18" s="85"/>
@@ -4874,7 +4877,7 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" s="11" customFormat="1">
       <c r="B19" s="12"/>
       <c r="C19" s="85"/>
       <c r="D19" s="85"/>
@@ -4884,7 +4887,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" s="11" customFormat="1">
       <c r="B20" s="12"/>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
@@ -4894,7 +4897,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" s="11" customFormat="1">
       <c r="B21" s="12"/>
       <c r="C21" s="86"/>
       <c r="D21" s="86"/>
@@ -4904,7 +4907,7 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" s="11" customFormat="1">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -4914,7 +4917,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="2:11" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" s="11" customFormat="1">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -4924,11 +4927,11 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="2:11" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" ht="15.75">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="79" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E24" s="79"/>
       <c r="F24" s="79"/>
@@ -4936,14 +4939,14 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>13</v>
@@ -4952,55 +4955,55 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="2:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="26.25" thickBot="1">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E28" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="52" t="s">
         <v>24</v>
-      </c>
-      <c r="F28" s="52" t="s">
-        <v>25</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" ht="13.5" thickTop="1">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="53">
         <v>700</v>
@@ -5012,11 +5015,11 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E30" s="30">
         <v>300</v>
@@ -5029,11 +5032,11 @@
       <c r="I30" s="12"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="13.5" thickBot="1">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E31" s="92">
         <v>500</v>
@@ -5043,7 +5046,7 @@
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="2:11" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -5053,7 +5056,7 @@
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" s="11" customFormat="1">
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
@@ -5063,7 +5066,7 @@
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" s="11" customFormat="1">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
@@ -5073,7 +5076,7 @@
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" s="11" customFormat="1">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -5083,7 +5086,7 @@
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -5093,10 +5096,10 @@
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="15" thickBot="1">
       <c r="B37" s="12"/>
       <c r="C37" s="87" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D37" s="87"/>
       <c r="E37" s="87"/>
@@ -5105,17 +5108,17 @@
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" s="11" customFormat="1">
       <c r="B38" s="12"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" s="11" customFormat="1">
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -5125,10 +5128,10 @@
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
-    <row r="40" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" s="11" customFormat="1">
       <c r="B40" s="12"/>
       <c r="C40" s="84" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D40" s="84"/>
       <c r="E40" s="84"/>
@@ -5137,7 +5140,7 @@
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
     </row>
-    <row r="41" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" s="11" customFormat="1">
       <c r="B41" s="12"/>
       <c r="C41" s="85"/>
       <c r="D41" s="85"/>
@@ -5147,7 +5150,7 @@
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
     </row>
-    <row r="42" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" s="11" customFormat="1">
       <c r="B42" s="12"/>
       <c r="C42" s="85"/>
       <c r="D42" s="85"/>
@@ -5157,7 +5160,7 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
     </row>
-    <row r="43" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" s="11" customFormat="1">
       <c r="B43" s="12"/>
       <c r="C43" s="86"/>
       <c r="D43" s="86"/>
@@ -5167,7 +5170,7 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
     </row>
-    <row r="44" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" s="11" customFormat="1">
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
@@ -5177,7 +5180,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
     </row>
-    <row r="45" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" s="11" customFormat="1">
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
@@ -5187,11 +5190,11 @@
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
     </row>
-    <row r="46" spans="2:9" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" s="11" customFormat="1" ht="15.75">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E46" s="79"/>
       <c r="F46" s="79"/>
@@ -5199,27 +5202,27 @@
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
     </row>
-    <row r="47" spans="2:9" s="11" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" s="11" customFormat="1" ht="26.25" thickBot="1">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E47" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="52" t="s">
         <v>24</v>
-      </c>
-      <c r="F47" s="52" t="s">
-        <v>25</v>
       </c>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
     </row>
-    <row r="48" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48" s="53">
         <v>700</v>
@@ -5231,11 +5234,11 @@
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
     </row>
-    <row r="49" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" s="11" customFormat="1">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E49" s="30">
         <v>300</v>
@@ -5247,11 +5250,11 @@
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
     </row>
-    <row r="50" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E50" s="90">
         <v>500</v>
@@ -5261,7 +5264,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
     </row>
-    <row r="51" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -5271,7 +5274,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
     </row>
-    <row r="52" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" s="11" customFormat="1">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -5281,10 +5284,10 @@
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
     </row>
-    <row r="53" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" s="11" customFormat="1">
       <c r="B53" s="12"/>
       <c r="C53" s="84" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="D53" s="84"/>
       <c r="E53" s="84"/>
@@ -5293,7 +5296,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
     </row>
-    <row r="54" spans="2:9" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" s="11" customFormat="1" ht="13.5" customHeight="1">
       <c r="B54" s="12"/>
       <c r="C54" s="86"/>
       <c r="D54" s="86"/>
@@ -5303,7 +5306,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
     </row>
-    <row r="55" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" s="11" customFormat="1">
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
@@ -5313,7 +5316,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
     </row>
-    <row r="56" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" s="11" customFormat="1">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
@@ -5323,7 +5326,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
     </row>
-    <row r="57" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" s="11" customFormat="1">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
@@ -5333,7 +5336,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
     </row>
-    <row r="58" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" s="11" customFormat="1">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -5343,7 +5346,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
     </row>
-    <row r="59" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
@@ -5353,10 +5356,10 @@
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
     </row>
-    <row r="60" spans="2:9" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" s="11" customFormat="1" ht="15" thickBot="1">
       <c r="B60" s="12"/>
       <c r="C60" s="87" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D60" s="87"/>
       <c r="E60" s="87"/>
@@ -5365,7 +5368,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
     </row>
-    <row r="61" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" s="11" customFormat="1">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
@@ -5375,7 +5378,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
     </row>
-    <row r="62" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" s="11" customFormat="1">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
@@ -5385,10 +5388,10 @@
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
     </row>
-    <row r="63" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" s="11" customFormat="1">
       <c r="B63" s="12"/>
       <c r="C63" s="84" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D63" s="84"/>
       <c r="E63" s="84"/>
@@ -5397,7 +5400,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
     </row>
-    <row r="64" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" s="11" customFormat="1">
       <c r="B64" s="12"/>
       <c r="C64" s="85"/>
       <c r="D64" s="85"/>
@@ -5407,7 +5410,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
     </row>
-    <row r="65" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" s="11" customFormat="1">
       <c r="B65" s="12"/>
       <c r="C65" s="86"/>
       <c r="D65" s="86"/>
@@ -5417,7 +5420,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
     </row>
-    <row r="66" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" s="11" customFormat="1">
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
@@ -5427,7 +5430,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
     </row>
-    <row r="67" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" s="11" customFormat="1">
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -5437,11 +5440,11 @@
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
     </row>
-    <row r="68" spans="2:9" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" s="11" customFormat="1" ht="15.75">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="79" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E68" s="79"/>
       <c r="F68" s="79"/>
@@ -5449,49 +5452,45 @@
       <c r="H68" s="79"/>
       <c r="I68" s="12"/>
     </row>
-    <row r="69" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" s="11" customFormat="1">
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="89" t="s">
+        <v>117</v>
+      </c>
+      <c r="E69" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E69" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="F69" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="G69" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="H69" s="58" t="s">
-        <v>60</v>
-      </c>
+      <c r="F69" s="94"/>
+      <c r="G69" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="H69" s="94"/>
       <c r="I69" s="12"/>
     </row>
-    <row r="70" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="89"/>
       <c r="E70" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="F70" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="G70" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="H70" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="F70" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="G70" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="H70" s="52" t="s">
-        <v>65</v>
-      </c>
       <c r="I70" s="12"/>
     </row>
-    <row r="71" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E71" s="53">
         <v>55150</v>
@@ -5507,11 +5506,11 @@
       </c>
       <c r="I71" s="12"/>
     </row>
-    <row r="72" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" s="11" customFormat="1">
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E72" s="30">
         <v>57150</v>
@@ -5527,11 +5526,11 @@
       </c>
       <c r="I72" s="12"/>
     </row>
-    <row r="73" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" s="11" customFormat="1">
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E73" s="32">
         <v>64400</v>
@@ -5547,11 +5546,11 @@
       </c>
       <c r="I73" s="12"/>
     </row>
-    <row r="74" spans="2:9" s="11" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E74" s="54">
         <v>90400</v>
@@ -5567,7 +5566,7 @@
       </c>
       <c r="I74" s="12"/>
     </row>
-    <row r="75" spans="2:9" s="11" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
@@ -5577,7 +5576,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="12"/>
     </row>
-    <row r="76" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" s="11" customFormat="1">
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -5587,7 +5586,7 @@
       <c r="H76" s="12"/>
       <c r="I76" s="12"/>
     </row>
-    <row r="77" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" s="11" customFormat="1">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
@@ -5597,7 +5596,7 @@
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
     </row>
-    <row r="78" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" s="11" customFormat="1">
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
@@ -5607,7 +5606,7 @@
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
     </row>
-    <row r="79" spans="2:9" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" s="11" customFormat="1" ht="15">
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="34" t="s">
@@ -5619,7 +5618,7 @@
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
     </row>
-    <row r="80" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" s="11" customFormat="1">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -5629,7 +5628,7 @@
       <c r="H80" s="12"/>
       <c r="I80" s="12"/>
     </row>
-    <row r="81" spans="2:9" s="11" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" s="11" customFormat="1">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -5640,7 +5639,7 @@
       <c r="I81" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="C60:F60"/>
     <mergeCell ref="C63:F65"/>
@@ -5655,6 +5654,8 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C40:F43"/>
     <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="G69:H69"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D79" location="_st3" tooltip="Step3. Examples of Decision Tables" display="Step 3."/>
@@ -5672,11 +5673,11 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C123" sqref="C123:F124"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
@@ -5690,7 +5691,7 @@
     <col min="10" max="10" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -5699,7 +5700,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -5708,10 +5709,10 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="18.75" thickBot="1">
       <c r="A3" s="8"/>
       <c r="B3" s="78" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
@@ -5721,7 +5722,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.5" thickTop="1">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -5731,7 +5732,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -5741,7 +5742,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -5753,7 +5754,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.5" thickBot="1">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -5765,10 +5766,10 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="B8" s="12"/>
       <c r="C8" s="80" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D8" s="80"/>
       <c r="E8" s="80"/>
@@ -5779,7 +5780,7 @@
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="13.5" thickBot="1">
       <c r="B9" s="12"/>
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
@@ -5791,7 +5792,7 @@
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -5803,7 +5804,7 @@
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -5815,10 +5816,10 @@
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="B12" s="12"/>
       <c r="C12" s="84" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
@@ -5829,7 +5830,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="8" customFormat="1">
       <c r="B13" s="12"/>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
@@ -5841,7 +5842,7 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="B14" s="12"/>
       <c r="C14" s="86"/>
       <c r="D14" s="86"/>
@@ -5853,7 +5854,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -5865,7 +5866,7 @@
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="8" customFormat="1">
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -5877,7 +5878,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" s="8" customFormat="1">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -5889,7 +5890,7 @@
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" s="8" customFormat="1">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
@@ -5901,7 +5902,7 @@
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -5913,33 +5914,33 @@
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="B20" s="12"/>
-      <c r="C20" s="96" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
+      <c r="C20" s="97" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" s="8" customFormat="1">
       <c r="B21" s="12"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -5951,10 +5952,10 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="2:11" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" ht="15.75">
       <c r="B23" s="12"/>
       <c r="C23" s="79" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D23" s="79"/>
       <c r="E23" s="79"/>
@@ -5965,7 +5966,7 @@
       <c r="J23" s="79"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11">
       <c r="B24" s="12"/>
       <c r="C24" s="13" t="s">
         <v>1</v>
@@ -5974,9 +5975,9 @@
         <v>3</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="59" t="s">
         <v>5</v>
       </c>
       <c r="G24" s="36">
@@ -5993,7 +5994,7 @@
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="13.5" thickBot="1">
       <c r="B25" s="12"/>
       <c r="C25" s="13" t="s">
         <v>2</v>
@@ -6002,13 +6003,13 @@
         <v>4</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="60" t="s">
         <v>6</v>
       </c>
       <c r="G25" s="36">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H25" s="37">
         <v>17</v>
@@ -6021,7 +6022,7 @@
       </c>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="14.25" thickTop="1" thickBot="1">
       <c r="B26" s="12"/>
       <c r="C26" s="35" t="s">
         <v>13</v>
@@ -6032,43 +6033,45 @@
       <c r="E26" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="66" t="s">
+      <c r="F26" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="62" t="s">
+      <c r="G26" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="63" t="s">
+      <c r="H26" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="63" t="s">
+      <c r="I26" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="64" t="s">
+      <c r="J26" s="63" t="s">
         <v>10</v>
       </c>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" ht="13.5" thickTop="1">
       <c r="B27" s="12"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" s="8" customFormat="1">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" s="8" customFormat="1">
       <c r="B29" s="12"/>
       <c r="C29" s="84" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D29" s="84"/>
       <c r="E29" s="84"/>
@@ -6079,7 +6082,7 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" s="8" customFormat="1">
       <c r="B30" s="12"/>
       <c r="C30" s="85"/>
       <c r="D30" s="85"/>
@@ -6091,7 +6094,7 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" s="8" customFormat="1">
       <c r="B31" s="12"/>
       <c r="C31" s="85"/>
       <c r="D31" s="85"/>
@@ -6103,7 +6106,7 @@
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" s="8" customFormat="1">
       <c r="B32" s="12"/>
       <c r="C32" s="85"/>
       <c r="D32" s="85"/>
@@ -6115,7 +6118,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" s="8" customFormat="1">
       <c r="B33" s="12"/>
       <c r="C33" s="86"/>
       <c r="D33" s="86"/>
@@ -6127,7 +6130,7 @@
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" s="8" customFormat="1">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
@@ -6139,7 +6142,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -6151,7 +6154,7 @@
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -6163,7 +6166,7 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="2:11" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11">
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -6175,7 +6178,7 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="13.5" thickBot="1">
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -6187,10 +6190,10 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="B39" s="12"/>
       <c r="C39" s="87" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D39" s="87"/>
       <c r="E39" s="87"/>
@@ -6201,19 +6204,19 @@
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" s="8" customFormat="1">
       <c r="B40" s="12"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11" s="8" customFormat="1">
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
@@ -6225,10 +6228,10 @@
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
     </row>
-    <row r="42" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:11" s="8" customFormat="1">
       <c r="B42" s="12"/>
       <c r="C42" s="84" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D42" s="84"/>
       <c r="E42" s="84"/>
@@ -6239,7 +6242,7 @@
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
     </row>
-    <row r="43" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" s="8" customFormat="1">
       <c r="B43" s="12"/>
       <c r="C43" s="85"/>
       <c r="D43" s="85"/>
@@ -6251,7 +6254,7 @@
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
     </row>
-    <row r="44" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" s="8" customFormat="1">
       <c r="B44" s="12"/>
       <c r="C44" s="85"/>
       <c r="D44" s="85"/>
@@ -6263,7 +6266,7 @@
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
     </row>
-    <row r="45" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" s="8" customFormat="1">
       <c r="B45" s="12"/>
       <c r="C45" s="85"/>
       <c r="D45" s="85"/>
@@ -6275,7 +6278,7 @@
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" s="8" customFormat="1">
       <c r="B46" s="12"/>
       <c r="C46" s="86"/>
       <c r="D46" s="86"/>
@@ -6287,7 +6290,7 @@
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" s="8" customFormat="1">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -6299,7 +6302,7 @@
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11" s="8" customFormat="1">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -6311,11 +6314,11 @@
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
     </row>
-    <row r="49" spans="2:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:11" s="8" customFormat="1" ht="15.75">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="79" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E49" s="79"/>
       <c r="F49" s="79"/>
@@ -6325,13 +6328,13 @@
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
     </row>
-    <row r="50" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:11" s="8" customFormat="1">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
-      <c r="D50" s="97" t="s">
+      <c r="D50" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="E50" s="97"/>
+      <c r="E50" s="98"/>
       <c r="F50" s="13" t="s">
         <v>13</v>
       </c>
@@ -6341,13 +6344,13 @@
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:11" s="8" customFormat="1">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
-      <c r="D51" s="97" t="s">
-        <v>73</v>
-      </c>
-      <c r="E51" s="97"/>
+      <c r="D51" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" s="98"/>
       <c r="F51" s="13" t="s">
         <v>14</v>
       </c>
@@ -6357,14 +6360,14 @@
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
     </row>
-    <row r="52" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:11" s="8" customFormat="1">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>11</v>
@@ -6375,7 +6378,7 @@
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
     </row>
-    <row r="53" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="31" t="s">
@@ -6393,7 +6396,7 @@
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="16">
@@ -6411,7 +6414,7 @@
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:11" s="8" customFormat="1">
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="17">
@@ -6429,7 +6432,7 @@
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:11" s="8" customFormat="1">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="17">
@@ -6447,7 +6450,7 @@
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="19">
@@ -6456,7 +6459,7 @@
       <c r="E57" s="19">
         <v>23</v>
       </c>
-      <c r="F57" s="65" t="s">
+      <c r="F57" s="64" t="s">
         <v>10</v>
       </c>
       <c r="G57" s="12"/>
@@ -6465,7 +6468,7 @@
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
     </row>
-    <row r="58" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -6477,7 +6480,7 @@
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
     </row>
-    <row r="59" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:11" s="8" customFormat="1">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
@@ -6489,7 +6492,7 @@
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
     </row>
-    <row r="60" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:11" s="8" customFormat="1">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
@@ -6501,7 +6504,7 @@
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
     </row>
-    <row r="61" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:11" s="8" customFormat="1">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
@@ -6513,7 +6516,7 @@
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
     </row>
-    <row r="62" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
@@ -6525,10 +6528,10 @@
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
     </row>
-    <row r="63" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="B63" s="12"/>
       <c r="C63" s="87" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D63" s="87"/>
       <c r="E63" s="87"/>
@@ -6539,19 +6542,19 @@
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
     </row>
-    <row r="64" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:11" s="8" customFormat="1">
       <c r="B64" s="12"/>
-      <c r="C64" s="69"/>
-      <c r="D64" s="69"/>
-      <c r="E64" s="69"/>
-      <c r="F64" s="69"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="67"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
     </row>
-    <row r="65" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:14" s="8" customFormat="1">
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
@@ -6563,10 +6566,10 @@
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
     </row>
-    <row r="66" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:14" s="8" customFormat="1">
       <c r="B66" s="12"/>
       <c r="C66" s="84" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D66" s="84"/>
       <c r="E66" s="84"/>
@@ -6577,7 +6580,7 @@
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
     </row>
-    <row r="67" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:14" s="8" customFormat="1">
       <c r="B67" s="12"/>
       <c r="C67" s="85"/>
       <c r="D67" s="85"/>
@@ -6589,7 +6592,7 @@
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
     </row>
-    <row r="68" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:14" s="8" customFormat="1">
       <c r="B68" s="12"/>
       <c r="C68" s="85"/>
       <c r="D68" s="85"/>
@@ -6601,7 +6604,7 @@
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
     </row>
-    <row r="69" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:14" s="8" customFormat="1">
       <c r="B69" s="12"/>
       <c r="C69" s="85"/>
       <c r="D69" s="85"/>
@@ -6613,7 +6616,7 @@
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
     </row>
-    <row r="70" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:14" s="8" customFormat="1">
       <c r="B70" s="12"/>
       <c r="C70" s="85"/>
       <c r="D70" s="85"/>
@@ -6625,7 +6628,7 @@
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
     </row>
-    <row r="71" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:14" s="8" customFormat="1">
       <c r="B71" s="12"/>
       <c r="C71" s="85"/>
       <c r="D71" s="85"/>
@@ -6637,7 +6640,7 @@
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
     </row>
-    <row r="72" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:14" s="8" customFormat="1">
       <c r="B72" s="12"/>
       <c r="C72" s="85"/>
       <c r="D72" s="85"/>
@@ -6649,7 +6652,7 @@
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
     </row>
-    <row r="73" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:14" s="8" customFormat="1">
       <c r="B73" s="12"/>
       <c r="C73" s="85"/>
       <c r="D73" s="85"/>
@@ -6661,7 +6664,7 @@
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
     </row>
-    <row r="74" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:14" s="8" customFormat="1">
       <c r="B74" s="12"/>
       <c r="C74" s="85"/>
       <c r="D74" s="85"/>
@@ -6674,7 +6677,7 @@
       <c r="K74" s="12"/>
       <c r="N74" s="41"/>
     </row>
-    <row r="75" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:14" s="8" customFormat="1">
       <c r="B75" s="12"/>
       <c r="C75" s="86"/>
       <c r="D75" s="86"/>
@@ -6686,7 +6689,7 @@
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
     </row>
-    <row r="76" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:14" s="8" customFormat="1">
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -6698,7 +6701,7 @@
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
     </row>
-    <row r="77" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:14" s="8" customFormat="1">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
@@ -6710,12 +6713,12 @@
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
     </row>
-    <row r="78" spans="2:14" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:14" s="8" customFormat="1" ht="15.75">
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="79" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F78" s="79"/>
       <c r="G78" s="12"/>
@@ -6724,7 +6727,7 @@
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
     </row>
-    <row r="79" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:14" s="8" customFormat="1">
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
@@ -6740,12 +6743,12 @@
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
     </row>
-    <row r="80" spans="2:14" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:14" s="8" customFormat="1">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
       <c r="E80" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F80" s="13" t="s">
         <v>14</v>
@@ -6756,12 +6759,12 @@
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
     </row>
-    <row r="81" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:11" s="8" customFormat="1">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
       <c r="E81" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F81" s="13" t="s">
         <v>11</v>
@@ -6772,12 +6775,12 @@
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
     </row>
-    <row r="82" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
       <c r="E82" s="31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F82" s="45" t="s">
         <v>12</v>
@@ -6788,12 +6791,12 @@
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
     </row>
-    <row r="83" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
       <c r="E83" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F83" s="46" t="s">
         <v>7</v>
@@ -6804,12 +6807,12 @@
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
     </row>
-    <row r="84" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:11" s="8" customFormat="1">
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
       <c r="E84" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F84" s="18" t="s">
         <v>8</v>
@@ -6820,12 +6823,12 @@
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
     </row>
-    <row r="85" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:11" s="8" customFormat="1">
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F85" s="18" t="s">
         <v>9</v>
@@ -6836,14 +6839,14 @@
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
     </row>
-    <row r="86" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
       <c r="E86" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F86" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="F86" s="64" t="s">
         <v>10</v>
       </c>
       <c r="G86" s="12"/>
@@ -6852,7 +6855,7 @@
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
     </row>
-    <row r="87" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -6864,7 +6867,7 @@
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
     </row>
-    <row r="88" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:11" s="8" customFormat="1">
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -6876,10 +6879,10 @@
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
     </row>
-    <row r="89" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:11" s="8" customFormat="1">
       <c r="B89" s="12"/>
       <c r="C89" s="84" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D89" s="84"/>
       <c r="E89" s="84"/>
@@ -6890,7 +6893,7 @@
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
     </row>
-    <row r="90" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:11" s="8" customFormat="1">
       <c r="B90" s="12"/>
       <c r="C90" s="85"/>
       <c r="D90" s="85"/>
@@ -6902,7 +6905,7 @@
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
     </row>
-    <row r="91" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:11" s="8" customFormat="1">
       <c r="B91" s="12"/>
       <c r="C91" s="86"/>
       <c r="D91" s="86"/>
@@ -6914,7 +6917,7 @@
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:11" s="8" customFormat="1">
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -6926,7 +6929,7 @@
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
     </row>
-    <row r="93" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:11" s="8" customFormat="1">
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -6938,12 +6941,12 @@
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
     </row>
-    <row r="94" spans="2:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:11" s="8" customFormat="1" ht="15.75">
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
       <c r="E94" s="79" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F94" s="79"/>
       <c r="G94" s="12"/>
@@ -6952,12 +6955,12 @@
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
     </row>
-    <row r="95" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B95" s="12"/>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
       <c r="E95" s="31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F95" s="45" t="s">
         <v>12</v>
@@ -6968,15 +6971,15 @@
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
     </row>
-    <row r="96" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
       <c r="E96" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F96" s="46" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
@@ -6984,15 +6987,15 @@
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
     </row>
-    <row r="97" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:11" s="8" customFormat="1">
       <c r="B97" s="12"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
       <c r="E97" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F97" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
@@ -7000,15 +7003,15 @@
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
     </row>
-    <row r="98" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:11" s="8" customFormat="1">
       <c r="B98" s="12"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
       <c r="E98" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F98" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
@@ -7016,15 +7019,15 @@
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
     </row>
-    <row r="99" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
       <c r="E99" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F99" s="65" t="s">
-        <v>86</v>
+        <v>74</v>
+      </c>
+      <c r="F99" s="64" t="s">
+        <v>82</v>
       </c>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
@@ -7032,7 +7035,7 @@
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
     </row>
-    <row r="100" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B100" s="12"/>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
@@ -7044,7 +7047,7 @@
       <c r="J100" s="12"/>
       <c r="K100" s="12"/>
     </row>
-    <row r="101" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:11" s="8" customFormat="1">
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
       <c r="D101" s="12"/>
@@ -7056,7 +7059,7 @@
       <c r="J101" s="12"/>
       <c r="K101" s="12"/>
     </row>
-    <row r="102" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:11" s="8" customFormat="1">
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
@@ -7068,7 +7071,7 @@
       <c r="J102" s="12"/>
       <c r="K102" s="12"/>
     </row>
-    <row r="103" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:11" s="8" customFormat="1">
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
@@ -7080,7 +7083,7 @@
       <c r="J103" s="12"/>
       <c r="K103" s="12"/>
     </row>
-    <row r="104" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
@@ -7092,33 +7095,33 @@
       <c r="J104" s="12"/>
       <c r="K104" s="12"/>
     </row>
-    <row r="105" spans="2:11" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:11" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="B105" s="12"/>
-      <c r="C105" s="96" t="s">
-        <v>87</v>
-      </c>
-      <c r="D105" s="96"/>
-      <c r="E105" s="96"/>
-      <c r="F105" s="96"/>
+      <c r="C105" s="97" t="s">
+        <v>83</v>
+      </c>
+      <c r="D105" s="97"/>
+      <c r="E105" s="97"/>
+      <c r="F105" s="97"/>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
       <c r="J105" s="12"/>
       <c r="K105" s="12"/>
     </row>
-    <row r="106" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:11" s="8" customFormat="1">
       <c r="B106" s="12"/>
-      <c r="C106" s="68"/>
-      <c r="D106" s="68"/>
-      <c r="E106" s="68"/>
-      <c r="F106" s="68"/>
+      <c r="C106" s="66"/>
+      <c r="D106" s="66"/>
+      <c r="E106" s="66"/>
+      <c r="F106" s="66"/>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="12"/>
       <c r="K106" s="12"/>
     </row>
-    <row r="107" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:11" s="8" customFormat="1">
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
@@ -7130,12 +7133,12 @@
       <c r="J107" s="12"/>
       <c r="K107" s="12"/>
     </row>
-    <row r="108" spans="2:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:11" s="8" customFormat="1" ht="15.75">
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
       <c r="E108" s="79" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F108" s="79"/>
       <c r="G108" s="12"/>
@@ -7144,7 +7147,7 @@
       <c r="J108" s="12"/>
       <c r="K108" s="12"/>
     </row>
-    <row r="109" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:11" s="8" customFormat="1">
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
       <c r="D109" s="12"/>
@@ -7152,7 +7155,7 @@
         <v>1</v>
       </c>
       <c r="F109" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
@@ -7160,15 +7163,15 @@
       <c r="J109" s="12"/>
       <c r="K109" s="12"/>
     </row>
-    <row r="110" spans="2:11" s="8" customFormat="1" ht="27" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:11" s="8" customFormat="1" ht="25.5">
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
       <c r="E110" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F110" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
@@ -7176,12 +7179,12 @@
       <c r="J110" s="12"/>
       <c r="K110" s="12"/>
     </row>
-    <row r="111" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:11" s="8" customFormat="1">
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
       <c r="D111" s="12"/>
       <c r="E111" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F111" s="13" t="s">
         <v>11</v>
@@ -7192,12 +7195,12 @@
       <c r="J111" s="12"/>
       <c r="K111" s="12"/>
     </row>
-    <row r="112" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
       <c r="E112" s="31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F112" s="45" t="s">
         <v>12</v>
@@ -7208,12 +7211,12 @@
       <c r="J112" s="12"/>
       <c r="K112" s="12"/>
     </row>
-    <row r="113" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
       <c r="E113" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F113" s="46" t="s">
         <v>7</v>
@@ -7224,12 +7227,12 @@
       <c r="J113" s="12"/>
       <c r="K113" s="12"/>
     </row>
-    <row r="114" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:11" s="8" customFormat="1">
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
       <c r="D114" s="12"/>
       <c r="E114" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F114" s="18" t="s">
         <v>8</v>
@@ -7240,12 +7243,12 @@
       <c r="J114" s="12"/>
       <c r="K114" s="12"/>
     </row>
-    <row r="115" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:11" s="8" customFormat="1">
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
       <c r="D115" s="12"/>
       <c r="E115" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F115" s="18" t="s">
         <v>9</v>
@@ -7256,14 +7259,14 @@
       <c r="J115" s="12"/>
       <c r="K115" s="12"/>
     </row>
-    <row r="116" spans="2:11" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:11" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
       <c r="D116" s="12"/>
       <c r="E116" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F116" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="F116" s="64" t="s">
         <v>10</v>
       </c>
       <c r="G116" s="12"/>
@@ -7272,7 +7275,7 @@
       <c r="J116" s="12"/>
       <c r="K116" s="12"/>
     </row>
-    <row r="117" spans="2:11" s="8" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:11" s="8" customFormat="1" ht="13.5" thickTop="1">
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
       <c r="D117" s="12"/>
@@ -7284,7 +7287,7 @@
       <c r="J117" s="12"/>
       <c r="K117" s="12"/>
     </row>
-    <row r="118" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:11" s="8" customFormat="1">
       <c r="B118" s="12"/>
       <c r="C118" s="12"/>
       <c r="D118" s="12"/>
@@ -7296,33 +7299,33 @@
       <c r="J118" s="12"/>
       <c r="K118" s="12"/>
     </row>
-    <row r="119" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:11" s="8" customFormat="1">
       <c r="B119" s="12"/>
-      <c r="C119" s="94" t="s">
-        <v>91</v>
-      </c>
-      <c r="D119" s="94"/>
-      <c r="E119" s="94"/>
-      <c r="F119" s="94"/>
+      <c r="C119" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="D119" s="95"/>
+      <c r="E119" s="95"/>
+      <c r="F119" s="95"/>
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
       <c r="I119" s="12"/>
       <c r="J119" s="12"/>
       <c r="K119" s="12"/>
     </row>
-    <row r="120" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:11" s="8" customFormat="1">
       <c r="B120" s="12"/>
-      <c r="C120" s="95"/>
-      <c r="D120" s="95"/>
-      <c r="E120" s="95"/>
-      <c r="F120" s="95"/>
+      <c r="C120" s="96"/>
+      <c r="D120" s="96"/>
+      <c r="E120" s="96"/>
+      <c r="F120" s="96"/>
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
       <c r="I120" s="12"/>
       <c r="J120" s="12"/>
       <c r="K120" s="12"/>
     </row>
-    <row r="121" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:11" s="8" customFormat="1">
       <c r="B121" s="12"/>
       <c r="C121" s="12"/>
       <c r="D121" s="12"/>
@@ -7334,7 +7337,7 @@
       <c r="J121" s="12"/>
       <c r="K121" s="12"/>
     </row>
-    <row r="122" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:11" s="8" customFormat="1">
       <c r="B122" s="12"/>
       <c r="C122" s="12"/>
       <c r="D122" s="12"/>
@@ -7346,33 +7349,33 @@
       <c r="J122" s="12"/>
       <c r="K122" s="12"/>
     </row>
-    <row r="123" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:11" s="8" customFormat="1">
       <c r="B123" s="12"/>
-      <c r="C123" s="94" t="s">
-        <v>117</v>
-      </c>
-      <c r="D123" s="94"/>
-      <c r="E123" s="94"/>
-      <c r="F123" s="94"/>
+      <c r="C123" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="D123" s="95"/>
+      <c r="E123" s="95"/>
+      <c r="F123" s="95"/>
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
       <c r="I123" s="12"/>
       <c r="J123" s="12"/>
       <c r="K123" s="12"/>
     </row>
-    <row r="124" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:11" s="8" customFormat="1">
       <c r="B124" s="12"/>
-      <c r="C124" s="95"/>
-      <c r="D124" s="95"/>
-      <c r="E124" s="95"/>
-      <c r="F124" s="95"/>
+      <c r="C124" s="96"/>
+      <c r="D124" s="96"/>
+      <c r="E124" s="96"/>
+      <c r="F124" s="96"/>
       <c r="G124" s="12"/>
       <c r="H124" s="12"/>
       <c r="I124" s="12"/>
       <c r="J124" s="12"/>
       <c r="K124" s="12"/>
     </row>
-    <row r="125" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:11" s="8" customFormat="1">
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
       <c r="D125" s="12"/>
@@ -7384,7 +7387,7 @@
       <c r="J125" s="12"/>
       <c r="K125" s="12"/>
     </row>
-    <row r="126" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:11" s="8" customFormat="1">
       <c r="B126" s="12"/>
       <c r="C126" s="12"/>
       <c r="D126" s="12"/>
@@ -7396,7 +7399,7 @@
       <c r="J126" s="12"/>
       <c r="K126" s="12"/>
     </row>
-    <row r="127" spans="2:11" s="8" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:11" s="8" customFormat="1">
       <c r="B127" s="12"/>
       <c r="C127" s="12"/>
       <c r="D127" s="12"/>

</xml_diff>